<commit_message>
fixed darkmode quote carousel section, Service section
</commit_message>
<xml_diff>
--- a/Mem-task.xlsx
+++ b/Mem-task.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admins\Documents\BC58\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admins\Documents\BC58\Bootstrap5\Capstone\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3849DF51-1079-43D8-B944-EE427C06E9D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B106FD5-EFF7-4C77-AFEE-46461BC4D81A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{7EA4537B-328F-483D-A67B-C1722A1F4EE4}"/>
+    <workbookView xWindow="1092" yWindow="1596" windowWidth="19824" windowHeight="8964" xr2:uid="{7EA4537B-328F-483D-A67B-C1722A1F4EE4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="24">
   <si>
     <t>Tasks Name</t>
   </si>
@@ -96,6 +96,9 @@
   </si>
   <si>
     <t xml:space="preserve">Number </t>
+  </si>
+  <si>
+    <t>Record Capstone</t>
   </si>
 </sst>
 </file>
@@ -141,7 +144,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -172,12 +175,6 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFAEABAB"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="5">
     <border>
@@ -251,7 +248,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -276,9 +273,6 @@
     </xf>
     <xf numFmtId="9" fontId="3" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -597,7 +591,7 @@
   <dimension ref="A1:S8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K11" sqref="K11"/>
+      <selection activeCell="L7" sqref="L7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -797,7 +791,7 @@
         <v>16</v>
       </c>
       <c r="P4" s="4" t="s">
-        <v>11</v>
+        <v>23</v>
       </c>
       <c r="Q4" s="5">
         <v>45190</v>
@@ -806,10 +800,10 @@
         <v>1</v>
       </c>
       <c r="S4" s="6" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:19" ht="24.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="4" t="s">
         <v>13</v>
       </c>
@@ -840,9 +834,23 @@
       <c r="L5" s="5">
         <v>45190</v>
       </c>
-      <c r="M5" s="9"/>
+      <c r="M5" s="8">
+        <v>1</v>
+      </c>
       <c r="N5" s="6" t="s">
         <v>16</v>
+      </c>
+      <c r="P5" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q5" s="5">
+        <v>45190</v>
+      </c>
+      <c r="R5" s="8">
+        <v>1</v>
+      </c>
+      <c r="S5" s="6" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:19" ht="24.6" thickBot="1" x14ac:dyDescent="0.35">

</xml_diff>